<commit_message>
Draft episode 07, new image file for the episode, and modified excel file for episode 04
</commit_message>
<xml_diff>
--- a/files/04-fake-metabolism.xlsx
+++ b/files/04-fake-metabolism.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Backup_halliday\Bio_RDM\Ed-DASH\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Ed-DASH\fair-bio-practice\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D908B7DC-B4EB-4A92-B063-861BACF2F4B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F557BF16-F381-41D0-BAD6-1689F545EDA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CE63AA3-0727-4508-A1BF-BFA8A07EBE47}"/>
+    <workbookView xWindow="22932" yWindow="1548" windowWidth="23256" windowHeight="12576" xr2:uid="{8CE63AA3-0727-4508-A1BF-BFA8A07EBE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
   <si>
     <t>Sample</t>
   </si>
@@ -122,12 +122,6 @@
     <t>C00369</t>
   </si>
   <si>
-    <t>C02094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C00697 </t>
-  </si>
-  <si>
     <t>Title:</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
   </si>
   <si>
     <t>+SUC</t>
-  </si>
-  <si>
-    <t>Metabolites reported per g of dry weight</t>
   </si>
   <si>
     <t>NA</t>
@@ -171,47 +162,56 @@
 (g)</t>
   </si>
   <si>
+    <t>10 mg sucrose per GM-agar</t>
+  </si>
+  <si>
+    <t>long days 18 h light</t>
+  </si>
+  <si>
+    <t>short days 6 h light</t>
+  </si>
+  <si>
+    <t>Study date range</t>
+  </si>
+  <si>
+    <t>2019-12-05 to 2020-01-05</t>
+  </si>
+  <si>
+    <t>Funder</t>
+  </si>
+  <si>
+    <t>dx.doi.org/10.17504/protocols.io.xxxxxxx</t>
+  </si>
+  <si>
+    <t>dx.doi.org/10.17504/protocols.io.xaxaxax</t>
+  </si>
+  <si>
+    <t>BBSRC-bogus-bogus-grant</t>
+  </si>
+  <si>
+    <t>Sosa M; Pintos A</t>
+  </si>
+  <si>
+    <t>Clock modulation of starch, pigments and nitrogen</t>
+  </si>
+  <si>
     <t>Starch 
-(mg/g)</t>
-  </si>
-  <si>
-    <t>β-caroten (µg/g)</t>
-  </si>
-  <si>
-    <t>Nitrogen (mg/g)</t>
-  </si>
-  <si>
-    <t>10 mg sucrose per GM-agar</t>
-  </si>
-  <si>
-    <t>long days 18 h light</t>
-  </si>
-  <si>
-    <t>short days 6 h light</t>
-  </si>
-  <si>
-    <t>Study date range</t>
-  </si>
-  <si>
-    <t>2019-12-05 to 2020-01-05</t>
-  </si>
-  <si>
-    <t>Funder</t>
-  </si>
-  <si>
-    <t>dx.doi.org/10.17504/protocols.io.xxxxxxx</t>
-  </si>
-  <si>
-    <t>dx.doi.org/10.17504/protocols.io.xaxaxax</t>
-  </si>
-  <si>
-    <t>BBSRC-bogus-bogus-grant</t>
-  </si>
-  <si>
-    <t>Sosa M; Pintos A</t>
-  </si>
-  <si>
-    <t>Clock modulation of starch, pigments and nitrogen</t>
+(mg/g FW)</t>
+  </si>
+  <si>
+    <t>Cholorophyll (mg/g FW)</t>
+  </si>
+  <si>
+    <t>Sucrose (mg/g FW)</t>
+  </si>
+  <si>
+    <t>Metabolites reported per g of fresh weight of 6-week-old plant leaf rosettes</t>
+  </si>
+  <si>
+    <t>C00089</t>
+  </si>
+  <si>
+    <t>C01793</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,58 +608,60 @@
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -668,10 +670,10 @@
         <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -685,25 +687,25 @@
         <v>2</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -714,7 +716,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -726,16 +728,16 @@
         <v>25</v>
       </c>
       <c r="G8">
-        <v>56</v>
+        <v>0.1206</v>
       </c>
       <c r="H8">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>1.2</v>
       </c>
       <c r="J8">
-        <v>50</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -746,7 +748,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -758,16 +760,16 @@
         <v>25</v>
       </c>
       <c r="G9">
-        <v>50</v>
+        <v>0.1275</v>
       </c>
       <c r="H9">
-        <v>108</v>
+        <v>6.5</v>
       </c>
       <c r="I9">
-        <v>7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J9">
-        <v>70</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -778,7 +780,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -790,16 +792,16 @@
         <v>25</v>
       </c>
       <c r="G10">
-        <v>60</v>
+        <v>0.28720000000000001</v>
       </c>
       <c r="H10">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>100</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -810,7 +812,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -822,16 +824,16 @@
         <v>25</v>
       </c>
       <c r="G11">
-        <v>80</v>
+        <v>0.15240000000000001</v>
       </c>
       <c r="H11">
-        <v>115</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>8</v>
-      </c>
-      <c r="J11" t="s">
-        <v>37</v>
+        <v>0.6</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -842,7 +844,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
@@ -854,16 +856,16 @@
         <v>25</v>
       </c>
       <c r="G12">
-        <v>65</v>
+        <v>0.20349999999999999</v>
       </c>
       <c r="H12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -874,7 +876,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -885,17 +887,17 @@
       <c r="F13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G13">
-        <v>58</v>
+      <c r="G13" t="s">
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -906,7 +908,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -917,17 +919,17 @@
       <c r="F14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G14">
-        <v>43</v>
+      <c r="G14" t="s">
+        <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -938,7 +940,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -949,17 +951,17 @@
       <c r="F15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G15">
-        <v>66</v>
+      <c r="G15" t="s">
+        <v>34</v>
       </c>
       <c r="H15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -970,7 +972,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -981,17 +983,17 @@
       <c r="F16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G16">
-        <v>82</v>
+      <c r="G16" t="s">
+        <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1002,7 +1004,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1013,17 +1015,17 @@
       <c r="F17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G17">
-        <v>68</v>
+      <c r="G17" t="s">
+        <v>34</v>
       </c>
       <c r="H17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1031,7 +1033,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1039,15 +1041,15 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more complete metaexample with real protocols
</commit_message>
<xml_diff>
--- a/files/04-fake-metabolism.xlsx
+++ b/files/04-fake-metabolism.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Ed-DASH\fair-bio-practice\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ed-dash\fair-bio-practice\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F557BF16-F381-41D0-BAD6-1689F545EDA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="1548" windowWidth="23256" windowHeight="12576" xr2:uid="{8CE63AA3-0727-4508-A1BF-BFA8A07EBE47}"/>
+    <workbookView xWindow="22935" yWindow="1545" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>Sample</t>
   </si>
@@ -180,15 +179,6 @@
     <t>Funder</t>
   </si>
   <si>
-    <t>dx.doi.org/10.17504/protocols.io.xxxxxxx</t>
-  </si>
-  <si>
-    <t>dx.doi.org/10.17504/protocols.io.xaxaxax</t>
-  </si>
-  <si>
-    <t>BBSRC-bogus-bogus-grant</t>
-  </si>
-  <si>
     <t>Sosa M; Pintos A</t>
   </si>
   <si>
@@ -212,12 +202,27 @@
   </si>
   <si>
     <t>C01793</t>
+  </si>
+  <si>
+    <t>BBSRC-BB-V030557-1</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/nprot.2006.232    https://doi.org/10.1038/nprot.2009.12</t>
+  </si>
+  <si>
+    <t>Percivals E-36L</t>
+  </si>
+  <si>
+    <t>Cabinet</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.21769/BioProtoc.126</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -269,10 +274,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -281,6 +285,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,11 +607,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266DC06A-DB10-4F34-83F2-D44839EE072B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,29 +627,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>45</v>
       </c>
       <c r="G3" t="s">
@@ -644,24 +657,24 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>56</v>
+      <c r="A6" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -670,52 +683,52 @@
         <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>54</v>
+      <c r="H7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D8" t="s">
@@ -741,13 +754,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D9" t="s">
@@ -773,13 +786,13 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D10" t="s">
@@ -805,13 +818,13 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D11" t="s">
@@ -837,13 +850,13 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D12" t="s">
@@ -861,21 +874,21 @@
       <c r="H12" t="s">
         <v>34</v>
       </c>
-      <c r="I12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" t="s">
-        <v>34</v>
+      <c r="I12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J12">
+        <v>1.7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D13" t="s">
@@ -887,27 +900,27 @@
       <c r="F13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" t="s">
-        <v>34</v>
+      <c r="G13">
+        <v>0.2104</v>
+      </c>
+      <c r="H13">
+        <v>6.2</v>
+      </c>
+      <c r="I13">
+        <v>1.3</v>
+      </c>
+      <c r="J13">
+        <v>2.1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D14" t="s">
@@ -919,27 +932,27 @@
       <c r="F14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" t="s">
-        <v>34</v>
+      <c r="G14">
+        <v>0.24349999999999999</v>
+      </c>
+      <c r="H14">
+        <v>7</v>
+      </c>
+      <c r="I14">
+        <v>1.2</v>
+      </c>
+      <c r="J14">
+        <v>1.9</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D15" t="s">
@@ -951,27 +964,27 @@
       <c r="F15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
-        <v>34</v>
+      <c r="G15">
+        <v>0.32129999999999997</v>
+      </c>
+      <c r="H15">
+        <v>5.8</v>
+      </c>
+      <c r="I15">
+        <v>1.1000000000000001</v>
       </c>
       <c r="J15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D16" t="s">
@@ -983,27 +996,27 @@
       <c r="F16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" t="s">
-        <v>34</v>
+      <c r="G16">
+        <v>0.2135</v>
+      </c>
+      <c r="H16">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I16">
+        <v>0.8</v>
+      </c>
+      <c r="J16">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D17" t="s">
@@ -1015,29 +1028,38 @@
       <c r="F17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" t="s">
-        <v>34</v>
-      </c>
+      <c r="G17">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="H17">
+        <v>5.9</v>
+      </c>
+      <c r="I17">
+        <v>0.9</v>
+      </c>
+      <c r="J17">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
       </c>
+      <c r="E19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
@@ -1045,7 +1067,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B21" t="s">

</xml_diff>

<commit_message>
Improved meta example in excel
</commit_message>
<xml_diff>
--- a/files/04-fake-metabolism.xlsx
+++ b/files/04-fake-metabolism.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="22935" yWindow="1545" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Intro" sheetId="1" r:id="rId1"/>
+    <sheet name="Intro-Color" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="68">
   <si>
     <t>Sample</t>
   </si>
@@ -217,13 +218,110 @@
   </si>
   <si>
     <t>https://doi.org/10.21769/BioProtoc.126</t>
+  </si>
+  <si>
+    <t>Contact:</t>
+  </si>
+  <si>
+    <t>Thee Bosss bio_rdm@ed.ac.uk</t>
+  </si>
+  <si>
+    <t>Timet Project</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Biomas
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(g)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Starch 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(mg/g FW)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sucrose (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mg/g FW</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cholorophyll (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mg/g FW</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,13 +351,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -274,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -292,6 +416,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -608,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,6 +772,9 @@
       <c r="B1" t="s">
         <v>49</v>
       </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -658,107 +800,84 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>27</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>28</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
         <v>54</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:10" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8">
-        <v>0.1206</v>
-      </c>
-      <c r="H8">
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <v>1.2</v>
-      </c>
-      <c r="J8">
-        <v>1.8</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>36</v>
@@ -773,30 +892,30 @@
         <v>25</v>
       </c>
       <c r="G9">
-        <v>0.1275</v>
+        <v>0.1206</v>
       </c>
       <c r="H9">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="I9">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="J9">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
@@ -805,30 +924,30 @@
         <v>25</v>
       </c>
       <c r="G10">
-        <v>0.28720000000000001</v>
+        <v>0.1275</v>
       </c>
       <c r="H10">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J10">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -837,30 +956,30 @@
         <v>25</v>
       </c>
       <c r="G11">
-        <v>0.15240000000000001</v>
+        <v>0.28720000000000001</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
@@ -869,56 +988,56 @@
         <v>25</v>
       </c>
       <c r="G12">
-        <v>0.20349999999999999</v>
-      </c>
-      <c r="H12" t="s">
-        <v>34</v>
+        <v>0.15240000000000001</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
       </c>
       <c r="I12">
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="J12">
-        <v>1.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13">
-        <v>0.2104</v>
-      </c>
-      <c r="H13">
-        <v>6.2</v>
+        <v>0.20349999999999999</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
       </c>
       <c r="I13">
-        <v>1.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J13">
-        <v>2.1</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>36</v>
@@ -933,30 +1052,30 @@
         <v>26</v>
       </c>
       <c r="G14">
-        <v>0.24349999999999999</v>
+        <v>0.2104</v>
       </c>
       <c r="H14">
-        <v>7</v>
+        <v>6.2</v>
       </c>
       <c r="I14">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="J14">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
         <v>23</v>
@@ -965,30 +1084,30 @@
         <v>26</v>
       </c>
       <c r="G15">
-        <v>0.32129999999999997</v>
+        <v>0.24349999999999999</v>
       </c>
       <c r="H15">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J15" t="s">
-        <v>34</v>
+        <v>1.2</v>
+      </c>
+      <c r="J15">
+        <v>1.9</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>23</v>
@@ -997,30 +1116,30 @@
         <v>26</v>
       </c>
       <c r="G16">
-        <v>0.2135</v>
+        <v>0.32129999999999997</v>
       </c>
       <c r="H16">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
       <c r="I16">
-        <v>0.8</v>
-      </c>
-      <c r="J16">
-        <v>2.2000000000000002</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -1029,50 +1148,589 @@
         <v>26</v>
       </c>
       <c r="G17">
+        <v>0.2135</v>
+      </c>
+      <c r="H17">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I17">
+        <v>0.8</v>
+      </c>
+      <c r="J17">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18">
         <v>0.29199999999999998</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>5.9</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>0.9</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>2.1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-    </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="A19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="F3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>0.1206</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>1.2</v>
+      </c>
+      <c r="J9">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>0.1275</v>
+      </c>
+      <c r="H10">
+        <v>6.5</v>
+      </c>
+      <c r="I10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J10">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12">
+        <v>0.15240000000000001</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>0.6</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13">
+        <v>0.20349999999999999</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J13">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14">
+        <v>0.2104</v>
+      </c>
+      <c r="H14">
+        <v>6.2</v>
+      </c>
+      <c r="I14">
+        <v>1.3</v>
+      </c>
+      <c r="J14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>0.24349999999999999</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>1.2</v>
+      </c>
+      <c r="J15">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16">
+        <v>0.32129999999999997</v>
+      </c>
+      <c r="H16">
+        <v>5.8</v>
+      </c>
+      <c r="I16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17">
+        <v>0.2135</v>
+      </c>
+      <c r="H17">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I17">
+        <v>0.8</v>
+      </c>
+      <c r="J17">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="H18">
+        <v>5.9</v>
+      </c>
+      <c r="I18">
+        <v>0.9</v>
+      </c>
+      <c r="J18">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="E20" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" s="11" t="s">
         <v>42</v>
       </c>
+      <c r="C22" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>